<commit_message>
Figure 5 ok now
</commit_message>
<xml_diff>
--- a/data/NGC253_HR/Results/Tables/SLIM_rings_average.xlsx
+++ b/data/NGC253_HR/Results/Tables/SLIM_rings_average.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frico/Documents/data/NGC253_HR/Results_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DA2708-BF55-AD40-A6A9-D4219C5FEBA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AC5C25-03C0-FF48-87F6-0409083D6DA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35040" yWindow="600" windowWidth="27240" windowHeight="16440" xr2:uid="{C19457A6-CD48-CF49-B2D4-65AE6EFB1932}"/>
+    <workbookView xWindow="34880" yWindow="1340" windowWidth="25600" windowHeight="16440" xr2:uid="{C19457A6-CD48-CF49-B2D4-65AE6EFB1932}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>dist_pc</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>logN_old</t>
+  </si>
+  <si>
+    <t>Tex_SM</t>
+  </si>
+  <si>
+    <t>Tex_SM_err</t>
+  </si>
+  <si>
+    <t>logN_SM</t>
+  </si>
+  <si>
+    <t>logN_SM_err</t>
+  </si>
+  <si>
+    <t>FWHM_SM</t>
+  </si>
+  <si>
+    <t>FWHM_SM_err</t>
   </si>
 </sst>
 </file>
@@ -96,8 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,619 +432,907 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F859D43A-6B0B-2C4F-B3B9-E94922507BE9}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.05</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
+        <v>750.93870000000004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>55.286793000000003</v>
+      </c>
+      <c r="D2" s="1">
+        <v>16.206199999999999</v>
+      </c>
+      <c r="E2">
+        <v>14.825100000000001</v>
+      </c>
+      <c r="F2">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
         <v>792.89980000000003</v>
       </c>
-      <c r="C2">
+      <c r="I2">
         <v>120</v>
       </c>
-      <c r="D2">
+      <c r="J2">
         <v>57.505713999999998</v>
       </c>
-      <c r="E2">
+      <c r="K2">
         <v>16.206199999999999</v>
       </c>
-      <c r="F2">
+      <c r="L2">
         <v>14.825100000000001</v>
       </c>
-      <c r="G2">
+      <c r="M2">
         <v>16.392752000000002</v>
       </c>
-      <c r="H2">
+      <c r="N2">
         <v>14.901296</v>
       </c>
-      <c r="I2">
+      <c r="O2">
         <v>51.549329999999998</v>
       </c>
-      <c r="J2">
+      <c r="P2">
         <v>3.2247461999999998</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>261.50943000000001</v>
       </c>
-      <c r="L2">
+      <c r="R2">
         <v>1.1649887999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0.15</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
+        <v>611.42052999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>33.956305999999998</v>
+      </c>
+      <c r="D3" s="1">
+        <v>16.372243000000001</v>
+      </c>
+      <c r="E3">
+        <v>14.784681000000001</v>
+      </c>
+      <c r="F3">
+        <v>34.895954000000003</v>
+      </c>
+      <c r="G3">
+        <v>2.0152771</v>
+      </c>
+      <c r="H3">
         <v>749.04485999999997</v>
       </c>
-      <c r="C3">
+      <c r="I3">
         <v>30.242432000000001</v>
       </c>
-      <c r="D3">
+      <c r="J3">
         <v>30.242432000000001</v>
       </c>
-      <c r="E3">
+      <c r="K3">
         <v>16.372243000000001</v>
       </c>
-      <c r="F3">
+      <c r="L3">
         <v>14.784681000000001</v>
       </c>
-      <c r="G3">
+      <c r="M3">
         <v>16.470686000000001</v>
       </c>
-      <c r="H3">
+      <c r="N3">
         <v>14.784681000000001</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>47.257846999999998</v>
       </c>
-      <c r="J3">
+      <c r="P3">
         <v>1.3314751</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>259.12423999999999</v>
       </c>
-      <c r="L3">
+      <c r="R3">
         <v>0.59904329999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0.25</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
+        <v>555.48490000000004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>24.707761999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>16.402992000000001</v>
+      </c>
+      <c r="E4">
+        <v>14.700161</v>
+      </c>
+      <c r="F4">
+        <v>33.04</v>
+      </c>
+      <c r="G4">
+        <v>1.7107022999999999</v>
+      </c>
+      <c r="H4">
         <v>533.02769999999998</v>
       </c>
-      <c r="C4">
+      <c r="I4">
         <v>14.564088</v>
       </c>
-      <c r="D4">
+      <c r="J4">
         <v>14.564088</v>
       </c>
-      <c r="E4">
+      <c r="K4">
         <v>16.402992000000001</v>
       </c>
-      <c r="F4">
+      <c r="L4">
         <v>14.700161</v>
       </c>
-      <c r="G4">
+      <c r="M4">
         <v>16.402992000000001</v>
       </c>
-      <c r="H4">
+      <c r="N4">
         <v>14.700161</v>
       </c>
-      <c r="I4">
+      <c r="O4">
         <v>38.341231999999998</v>
       </c>
-      <c r="J4">
+      <c r="P4">
         <v>0.7584457</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>256.10473999999999</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <v>0.35189619999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.35</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
+        <v>504.92079999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>25.675034</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.387295000000002</v>
+      </c>
+      <c r="E5">
+        <v>14.583663</v>
+      </c>
+      <c r="F5">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
         <v>518.25409999999999</v>
       </c>
-      <c r="C5">
+      <c r="I5">
         <v>11.486844</v>
       </c>
-      <c r="D5">
+      <c r="J5">
         <v>11.486844</v>
       </c>
-      <c r="E5">
+      <c r="K5">
         <v>16.387295000000002</v>
       </c>
-      <c r="F5">
+      <c r="L5">
         <v>14.583663</v>
       </c>
-      <c r="G5">
+      <c r="M5">
         <v>16.387295000000002</v>
       </c>
-      <c r="H5">
+      <c r="N5">
         <v>14.583663</v>
       </c>
-      <c r="I5">
+      <c r="O5">
         <v>38.843204</v>
       </c>
-      <c r="J5">
+      <c r="P5">
         <v>0.60836214</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>253.76324</v>
       </c>
-      <c r="L5">
+      <c r="R5">
         <v>0.28097307999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.45</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
+        <v>419.82600000000002</v>
+      </c>
+      <c r="C6" s="2">
+        <v>37.043700000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16.21133</v>
+      </c>
+      <c r="E6">
+        <v>14.561722</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>-1</v>
+      </c>
+      <c r="H6">
         <v>447.81137000000001</v>
       </c>
-      <c r="C6">
+      <c r="I6">
         <v>12.255432000000001</v>
       </c>
-      <c r="D6">
+      <c r="J6">
         <v>12.255432000000001</v>
       </c>
-      <c r="E6">
+      <c r="K6">
         <v>16.279910000000001</v>
       </c>
-      <c r="F6">
+      <c r="L6">
         <v>14.561722</v>
       </c>
-      <c r="G6">
+      <c r="M6">
         <v>16.279910000000001</v>
       </c>
-      <c r="H6">
+      <c r="N6">
         <v>14.561722</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>36.559666</v>
       </c>
-      <c r="J6">
+      <c r="P6">
         <v>0.63371699999999997</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>252.67286999999999</v>
       </c>
-      <c r="L6">
+      <c r="R6">
         <v>0.2922535</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
+        <v>383.87299999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>35.112000000000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>16.040030999999999</v>
+      </c>
+      <c r="E7">
+        <v>14.669394499999999</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
         <v>371.81639999999999</v>
       </c>
-      <c r="C7">
+      <c r="I7">
         <v>14.831856999999999</v>
       </c>
-      <c r="D7">
+      <c r="J7">
         <v>14.831856999999999</v>
       </c>
-      <c r="E7">
+      <c r="K7">
         <v>16.121314999999999</v>
       </c>
-      <c r="F7">
+      <c r="L7">
         <v>14.669394499999999</v>
       </c>
-      <c r="G7">
+      <c r="M7">
         <v>16.121314999999999</v>
       </c>
-      <c r="H7">
+      <c r="N7">
         <v>14.669394499999999</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>31.875865999999998</v>
       </c>
-      <c r="J7">
+      <c r="P7">
         <v>0.83089389999999996</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>252.23811000000001</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <v>0.37511699999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.65</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
+        <v>357.31900000000002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>33.753</v>
+      </c>
+      <c r="D8" s="1">
+        <v>15.916852</v>
+      </c>
+      <c r="E8">
+        <v>14.184642</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
         <v>350.99624999999997</v>
       </c>
-      <c r="C8">
+      <c r="I8">
         <v>9.0922099999999997</v>
       </c>
-      <c r="D8">
+      <c r="J8">
         <v>9.0922099999999997</v>
       </c>
-      <c r="E8">
+      <c r="K8">
         <v>15.908402000000001</v>
       </c>
-      <c r="F8">
+      <c r="L8">
         <v>14.184642</v>
       </c>
-      <c r="G8">
+      <c r="M8">
         <v>15.908402000000001</v>
       </c>
-      <c r="H8">
+      <c r="N8">
         <v>14.184642</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>30.819762999999998</v>
       </c>
-      <c r="J8">
+      <c r="P8">
         <v>0.6680606</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>253.67401000000001</v>
       </c>
-      <c r="L8">
+      <c r="R8">
         <v>0.29033372000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.75</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
+        <v>279.8107</v>
+      </c>
+      <c r="C9" s="2">
+        <v>30.169988</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15.705764</v>
+      </c>
+      <c r="E9">
+        <v>14.144581000000001</v>
+      </c>
+      <c r="F9">
+        <v>26.18252</v>
+      </c>
+      <c r="G9">
+        <v>0.85254836000000001</v>
+      </c>
+      <c r="H9">
         <v>260.65102999999999</v>
       </c>
-      <c r="C9">
+      <c r="I9">
         <v>8.8335050000000006</v>
       </c>
-      <c r="D9">
+      <c r="J9">
         <v>8.8335050000000006</v>
       </c>
-      <c r="E9">
+      <c r="K9">
         <v>15.701473999999999</v>
       </c>
-      <c r="F9">
+      <c r="L9">
         <v>14.089874999999999</v>
       </c>
-      <c r="G9">
+      <c r="M9">
         <v>15.701473999999999</v>
       </c>
-      <c r="H9">
+      <c r="N9">
         <v>14.089874999999999</v>
       </c>
-      <c r="I9">
+      <c r="O9">
         <v>26.890446000000001</v>
       </c>
-      <c r="J9">
+      <c r="P9">
         <v>0.76043205999999997</v>
       </c>
-      <c r="K9">
+      <c r="Q9">
         <v>254.8312</v>
       </c>
-      <c r="L9">
+      <c r="R9">
         <v>0.32830045000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.85</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
+        <v>227.76087999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20.776796000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>15.581820499999999</v>
+      </c>
+      <c r="E10">
+        <v>14.105649</v>
+      </c>
+      <c r="F10">
+        <v>27.170921</v>
+      </c>
+      <c r="G10">
+        <v>1.0321518999999999</v>
+      </c>
+      <c r="H10">
         <v>203.44458</v>
       </c>
-      <c r="C10">
+      <c r="I10">
         <v>9.6998499999999996</v>
       </c>
-      <c r="D10">
+      <c r="J10">
         <v>9.6998499999999996</v>
       </c>
-      <c r="E10">
+      <c r="K10">
         <v>15.569924</v>
       </c>
-      <c r="F10">
+      <c r="L10">
         <v>14.066254000000001</v>
       </c>
-      <c r="G10">
+      <c r="M10">
         <v>15.569924</v>
       </c>
-      <c r="H10">
+      <c r="N10">
         <v>14.066254000000001</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>27.238726</v>
       </c>
-      <c r="J10">
+      <c r="P10">
         <v>0.97125936000000002</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
         <v>255.44872000000001</v>
       </c>
-      <c r="L10">
+      <c r="R10">
         <v>0.42034924000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.95</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
+        <v>213.71396999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>22.269746000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>15.460145000000001</v>
+      </c>
+      <c r="E11">
+        <v>14.0542555</v>
+      </c>
+      <c r="F11">
+        <v>28.15175</v>
+      </c>
+      <c r="G11">
+        <v>1.2572781</v>
+      </c>
+      <c r="H11">
         <v>149.13416000000001</v>
       </c>
-      <c r="C11">
-        <v>-10</v>
-      </c>
-      <c r="D11">
-        <v>-10</v>
-      </c>
-      <c r="E11">
+      <c r="I11">
+        <v>-10</v>
+      </c>
+      <c r="J11">
+        <v>-10</v>
+      </c>
+      <c r="K11">
         <v>15.453155000000001</v>
       </c>
-      <c r="F11">
+      <c r="L11">
         <v>13.990188</v>
       </c>
-      <c r="G11">
+      <c r="M11">
         <v>15.453155000000001</v>
       </c>
-      <c r="H11">
+      <c r="N11">
         <v>13.990188</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>29.32</v>
       </c>
-      <c r="J11">
+      <c r="P11">
         <v>1.0923</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
         <v>255.63835</v>
       </c>
-      <c r="L11">
+      <c r="R11">
         <v>0.57303340000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.05</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
+        <v>185.85380000000001</v>
+      </c>
+      <c r="C12">
+        <v>-10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>15.230821000000001</v>
+      </c>
+      <c r="E12">
+        <v>13.960091</v>
+      </c>
+      <c r="F12">
+        <v>24.12341</v>
+      </c>
+      <c r="G12">
+        <v>0.62569240000000004</v>
+      </c>
+      <c r="H12">
         <v>167.22037</v>
       </c>
-      <c r="C12">
-        <v>-10</v>
-      </c>
-      <c r="D12">
-        <v>-10</v>
-      </c>
-      <c r="E12">
+      <c r="I12">
+        <v>-10</v>
+      </c>
+      <c r="J12">
+        <v>-10</v>
+      </c>
+      <c r="K12">
         <v>15.235281000000001</v>
       </c>
-      <c r="F12">
+      <c r="L12">
         <v>13.931760000000001</v>
       </c>
-      <c r="G12">
+      <c r="M12">
         <v>15.235281000000001</v>
       </c>
-      <c r="H12">
+      <c r="N12">
         <v>13.931760000000001</v>
       </c>
-      <c r="I12">
+      <c r="O12">
         <v>24.504062999999999</v>
       </c>
-      <c r="J12">
+      <c r="P12">
         <v>1.3922833999999999</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>255.57740000000001</v>
       </c>
-      <c r="L12">
+      <c r="R12">
         <v>0.59941440000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1.1499999999999999</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
+        <v>185.85380000000001</v>
+      </c>
+      <c r="C13">
+        <v>-10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>15.134985</v>
+      </c>
+      <c r="E13">
+        <v>13.933128999999999</v>
+      </c>
+      <c r="F13">
+        <v>24.410156000000001</v>
+      </c>
+      <c r="G13">
+        <v>1.7580484999999999</v>
+      </c>
+      <c r="H13">
         <v>173.17116999999999</v>
       </c>
-      <c r="C13">
-        <v>-10</v>
-      </c>
-      <c r="D13">
-        <v>-10</v>
-      </c>
-      <c r="E13">
+      <c r="I13">
+        <v>-10</v>
+      </c>
+      <c r="J13">
+        <v>-10</v>
+      </c>
+      <c r="K13">
         <v>15.1298485</v>
       </c>
-      <c r="F13">
+      <c r="L13">
         <v>13.903575999999999</v>
       </c>
-      <c r="G13">
+      <c r="M13">
         <v>15.1298485</v>
       </c>
-      <c r="H13">
+      <c r="N13">
         <v>13.903575999999999</v>
       </c>
-      <c r="I13">
+      <c r="O13">
         <v>24.369378999999999</v>
       </c>
-      <c r="J13">
+      <c r="P13">
         <v>1.6586485</v>
       </c>
-      <c r="K13">
+      <c r="Q13">
         <v>254.86864</v>
       </c>
-      <c r="L13">
+      <c r="R13">
         <v>0.71172714000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1.25</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
+        <v>185.85380000000001</v>
+      </c>
+      <c r="C14">
+        <v>-10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>15.108110999999999</v>
+      </c>
+      <c r="E14">
+        <v>13.914001000000001</v>
+      </c>
+      <c r="F14">
+        <v>25.711400999999999</v>
+      </c>
+      <c r="G14">
+        <v>1.8817493000000001</v>
+      </c>
+      <c r="H14">
         <v>163.381</v>
       </c>
-      <c r="C14">
-        <v>-10</v>
-      </c>
-      <c r="D14">
-        <v>-10</v>
-      </c>
-      <c r="E14">
+      <c r="I14">
+        <v>-10</v>
+      </c>
+      <c r="J14">
+        <v>-10</v>
+      </c>
+      <c r="K14">
         <v>15.108110999999999</v>
       </c>
-      <c r="F14">
+      <c r="L14">
         <v>13.914001000000001</v>
       </c>
-      <c r="G14">
+      <c r="M14">
         <v>15.108110999999999</v>
       </c>
-      <c r="H14">
+      <c r="N14">
         <v>13.914001000000001</v>
       </c>
-      <c r="I14">
+      <c r="O14">
         <v>25.711400999999999</v>
       </c>
-      <c r="J14">
+      <c r="P14">
         <v>1.8817493000000001</v>
       </c>
-      <c r="K14">
+      <c r="Q14">
         <v>254.64293000000001</v>
       </c>
-      <c r="L14">
+      <c r="R14">
         <v>0.80727833999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1.35</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
+        <v>185.85380000000001</v>
+      </c>
+      <c r="C15">
+        <v>-10</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15.071222000000001</v>
+      </c>
+      <c r="E15">
+        <v>13.898539</v>
+      </c>
+      <c r="F15">
+        <v>29.085802000000001</v>
+      </c>
+      <c r="G15">
+        <v>2.2470043</v>
+      </c>
+      <c r="H15">
         <v>167.78531000000001</v>
       </c>
-      <c r="C15">
-        <v>-10</v>
-      </c>
-      <c r="D15">
-        <v>-10</v>
-      </c>
-      <c r="E15">
+      <c r="I15">
+        <v>-10</v>
+      </c>
+      <c r="J15">
+        <v>-10</v>
+      </c>
+      <c r="K15">
         <v>15.071222000000001</v>
       </c>
-      <c r="F15">
+      <c r="L15">
         <v>13.898539</v>
       </c>
-      <c r="G15">
+      <c r="M15">
         <v>15.071222000000001</v>
       </c>
-      <c r="H15">
+      <c r="N15">
         <v>13.898539</v>
       </c>
-      <c r="I15">
+      <c r="O15">
         <v>29.085802000000001</v>
       </c>
-      <c r="J15">
+      <c r="P15">
         <v>2.2470043</v>
       </c>
-      <c r="K15">
+      <c r="Q15">
         <v>252.17354</v>
       </c>
-      <c r="L15">
+      <c r="R15">
         <v>0.96184974999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1.45</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
+        <v>185.85380000000001</v>
+      </c>
+      <c r="C16">
+        <v>-10</v>
+      </c>
+      <c r="D16" s="1">
+        <v>15.051966999999999</v>
+      </c>
+      <c r="E16">
+        <v>13.878314</v>
+      </c>
+      <c r="F16">
+        <v>27.467617000000001</v>
+      </c>
+      <c r="G16">
+        <v>2.0768491999999998</v>
+      </c>
+      <c r="H16">
         <v>146.69999999999999</v>
       </c>
-      <c r="C16">
-        <v>-10</v>
-      </c>
-      <c r="D16">
-        <v>-10</v>
-      </c>
-      <c r="E16">
+      <c r="I16">
+        <v>-10</v>
+      </c>
+      <c r="J16">
+        <v>-10</v>
+      </c>
+      <c r="K16">
         <v>15.051966999999999</v>
       </c>
-      <c r="F16">
+      <c r="L16">
         <v>13.878314</v>
       </c>
-      <c r="G16">
+      <c r="M16">
         <v>15.051966999999999</v>
       </c>
-      <c r="H16">
+      <c r="N16">
         <v>13.878314</v>
       </c>
-      <c r="I16">
+      <c r="O16">
         <v>27.467617000000001</v>
       </c>
-      <c r="J16">
+      <c r="P16">
         <v>2.0768491999999998</v>
       </c>
-      <c r="K16">
+      <c r="Q16">
         <v>252.06439</v>
       </c>
-      <c r="L16">
+      <c r="R16">
         <v>0.89040344999999999</v>
       </c>
     </row>

</xml_diff>